<commit_message>
second pc tested. remaining 1
</commit_message>
<xml_diff>
--- a/Documentation/Resultados.xlsx
+++ b/Documentation/Resultados.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\1143875103\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aee759da35fbf519/Universidad/Carrera/Programacion/Visual C^N/WorkShop_SortExperiment/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_B47ED00D4EE572435E31B354240A8BC05D9E4E88" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4C6F7D66-4E98-4983-9178-2D77A6F55CB5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="22">
   <si>
     <t>3.2 Ghz</t>
   </si>
@@ -87,12 +88,15 @@
   </si>
   <si>
     <t>RadixSort 3.3</t>
+  </si>
+  <si>
+    <t>1.6 Ghz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,10 +140,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,59 +423,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -481,11 +485,14 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
+      <c r="E3">
+        <v>18151</v>
+      </c>
       <c r="G3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -495,11 +502,14 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
+      <c r="E4">
+        <v>67</v>
+      </c>
       <c r="G4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -509,11 +519,14 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
       <c r="G5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -523,11 +536,14 @@
       <c r="D6" t="s">
         <v>6</v>
       </c>
+      <c r="E6">
+        <v>470</v>
+      </c>
       <c r="G6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -537,11 +553,14 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
+      <c r="E7">
+        <v>434</v>
+      </c>
       <c r="G7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -551,11 +570,14 @@
       <c r="D8" t="s">
         <v>8</v>
       </c>
+      <c r="E8">
+        <v>382</v>
+      </c>
       <c r="G8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -565,11 +587,14 @@
       <c r="D9" t="s">
         <v>9</v>
       </c>
+      <c r="E9">
+        <v>26654</v>
+      </c>
       <c r="G9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -579,11 +604,14 @@
       <c r="D10" t="s">
         <v>10</v>
       </c>
+      <c r="E10">
+        <v>51865</v>
+      </c>
       <c r="G10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -593,11 +621,14 @@
       <c r="D11" t="s">
         <v>11</v>
       </c>
+      <c r="E11">
+        <v>33492</v>
+      </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -607,11 +638,14 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
+      <c r="E12">
+        <v>8854</v>
+      </c>
       <c r="G12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -621,11 +655,14 @@
       <c r="D13" t="s">
         <v>13</v>
       </c>
+      <c r="E13">
+        <v>66</v>
+      </c>
       <c r="G13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -635,12 +672,14 @@
       <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>64</v>
+      </c>
       <c r="G14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -650,11 +689,14 @@
       <c r="D15" t="s">
         <v>15</v>
       </c>
+      <c r="E15">
+        <v>4147</v>
+      </c>
       <c r="G15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -664,11 +706,14 @@
       <c r="D16" t="s">
         <v>16</v>
       </c>
+      <c r="E16">
+        <v>5769</v>
+      </c>
       <c r="G16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -678,11 +723,14 @@
       <c r="D17" t="s">
         <v>17</v>
       </c>
+      <c r="E17">
+        <v>4252</v>
+      </c>
       <c r="G17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -692,11 +740,14 @@
       <c r="D18" t="s">
         <v>18</v>
       </c>
+      <c r="E18">
+        <v>672109</v>
+      </c>
       <c r="G18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -706,11 +757,14 @@
       <c r="D19" t="s">
         <v>19</v>
       </c>
+      <c r="E19">
+        <v>622476</v>
+      </c>
       <c r="G19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -720,15 +774,18 @@
       <c r="D20" t="s">
         <v>20</v>
       </c>
+      <c r="E20">
+        <v>363866</v>
+      </c>
       <c r="G20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
     </row>
   </sheetData>

</xml_diff>